<commit_message>
sort a report by ser+deser ops/sec
</commit_message>
<xml_diff>
--- a/GLD.SerializerBenchmark/Analysis.xlsx
+++ b/GLD.SerializerBenchmark/Analysis.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="SerializerBenchmark_Log" localSheetId="2">Sheet1!$A$1:$L$43</definedName>
+    <definedName name="SerializerBenchmark_Log" localSheetId="2">Sheet1!$A$1:$L$61</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="41">
   <si>
     <t>string</t>
   </si>
@@ -169,13 +169,7 @@
     <t>EDI_X12_835 No Atributes</t>
   </si>
   <si>
-    <t>Telemetry</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>SharpSerializer</t>
+    <t>ObjectGraph</t>
   </si>
 </sst>
 </file>
@@ -778,12 +772,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="46350720"/>
-        <c:axId val="46352256"/>
-        <c:axId val="38749056"/>
+        <c:axId val="169525248"/>
+        <c:axId val="169526784"/>
+        <c:axId val="63591744"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="46350720"/>
+        <c:axId val="169525248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46352256"/>
+        <c:crossAx val="169526784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -800,7 +794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46352256"/>
+        <c:axId val="169526784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,12 +805,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46350720"/>
+        <c:crossAx val="169525248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="38749056"/>
+        <c:axId val="63591744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +819,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46352256"/>
+        <c:crossAx val="169526784"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1783,12 +1777,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="46738432"/>
-        <c:axId val="46748416"/>
-        <c:axId val="38752704"/>
+        <c:axId val="170572416"/>
+        <c:axId val="170586496"/>
+        <c:axId val="64737280"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="46738432"/>
+        <c:axId val="170572416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1797,7 +1791,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46748416"/>
+        <c:crossAx val="170586496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1805,7 +1799,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46748416"/>
+        <c:axId val="170586496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,12 +1810,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46738432"/>
+        <c:crossAx val="170572416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="38752704"/>
+        <c:axId val="64737280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,7 +1824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46748416"/>
+        <c:crossAx val="170586496"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1867,15 +1861,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>119061</xdr:colOff>
+      <xdr:colOff>290511</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1935,7 +1929,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ganeline, Leonid" refreshedDate="42247.527995023149" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="3338">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L43" sheet="Sheet1"/>
+    <worksheetSource ref="A1:L61" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="StringOrStream" numFmtId="0">
@@ -49861,8 +49855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51435,11 +51429,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H72" sqref="H72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51448,10 +51442,10 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -51510,28 +51504,28 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F2" s="5">
-        <v>281923</v>
+        <v>34333</v>
       </c>
       <c r="G2" s="5">
-        <v>207660</v>
+        <v>17307</v>
       </c>
       <c r="H2" s="5">
-        <v>2065</v>
+        <v>24128</v>
       </c>
       <c r="I2" s="5">
-        <v>489583</v>
+        <v>51640</v>
       </c>
       <c r="J2" s="5">
-        <v>35</v>
+        <v>291</v>
       </c>
       <c r="K2" s="5">
-        <v>48</v>
+        <v>577</v>
       </c>
       <c r="L2" s="5">
-        <v>20</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -51548,28 +51542,28 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F3" s="5">
-        <v>20985</v>
+        <v>73159</v>
       </c>
       <c r="G3" s="5">
-        <v>22016</v>
+        <v>59435</v>
       </c>
       <c r="H3" s="5">
-        <v>2046</v>
+        <v>43556</v>
       </c>
       <c r="I3" s="5">
-        <v>43001</v>
+        <v>132594</v>
       </c>
       <c r="J3" s="5">
-        <v>476</v>
+        <v>136</v>
       </c>
       <c r="K3" s="5">
-        <v>454</v>
+        <v>168</v>
       </c>
       <c r="L3" s="5">
-        <v>232</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -51583,31 +51577,31 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F4" s="5">
-        <v>340</v>
+        <v>76645</v>
       </c>
       <c r="G4" s="5">
-        <v>290</v>
+        <v>128824</v>
       </c>
       <c r="H4" s="5">
-        <v>2065</v>
+        <v>100127</v>
       </c>
       <c r="I4" s="5">
-        <v>630</v>
+        <v>205469</v>
       </c>
       <c r="J4" s="5">
-        <v>29411</v>
+        <v>130</v>
       </c>
       <c r="K4" s="5">
-        <v>34482</v>
+        <v>77</v>
       </c>
       <c r="L4" s="5">
-        <v>15873</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -51621,31 +51615,31 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F5" s="5">
-        <v>351</v>
+        <v>808218</v>
       </c>
       <c r="G5" s="5">
-        <v>301</v>
+        <v>3227179</v>
       </c>
       <c r="H5" s="5">
-        <v>2046</v>
+        <v>100127</v>
       </c>
       <c r="I5" s="5">
-        <v>652</v>
+        <v>4035397</v>
       </c>
       <c r="J5" s="5">
-        <v>28490</v>
+        <v>12</v>
       </c>
       <c r="K5" s="5">
-        <v>33222</v>
+        <v>3</v>
       </c>
       <c r="L5" s="5">
-        <v>15337</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -51659,31 +51653,31 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="5">
-        <v>204</v>
+        <v>63965</v>
       </c>
       <c r="G6" s="5">
-        <v>215</v>
+        <v>18161</v>
       </c>
       <c r="H6" s="5">
-        <v>2065</v>
+        <v>48468</v>
       </c>
       <c r="I6" s="5">
-        <v>419</v>
+        <v>82126</v>
       </c>
       <c r="J6" s="5">
-        <v>49019</v>
+        <v>156</v>
       </c>
       <c r="K6" s="5">
-        <v>46511</v>
+        <v>550</v>
       </c>
       <c r="L6" s="5">
-        <v>23866</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -51697,36 +51691,36 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5">
-        <v>178</v>
+        <v>184517</v>
       </c>
       <c r="G7" s="5">
-        <v>360</v>
+        <v>44623</v>
       </c>
       <c r="H7" s="5">
-        <v>2046</v>
+        <v>15032</v>
       </c>
       <c r="I7" s="5">
-        <v>538</v>
+        <v>229140</v>
       </c>
       <c r="J7" s="5">
-        <v>56179</v>
+        <v>54</v>
       </c>
       <c r="K7" s="5">
-        <v>27777</v>
+        <v>224</v>
       </c>
       <c r="L7" s="5">
-        <v>18587</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -51735,36 +51729,36 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5">
-        <v>993</v>
+        <v>2749</v>
       </c>
       <c r="G8" s="5">
-        <v>1217</v>
+        <v>2580</v>
       </c>
       <c r="H8" s="5">
-        <v>2065</v>
+        <v>24128</v>
       </c>
       <c r="I8" s="5">
-        <v>2210</v>
+        <v>5329</v>
       </c>
       <c r="J8" s="5">
-        <v>10070</v>
+        <v>3637</v>
       </c>
       <c r="K8" s="5">
-        <v>8216</v>
+        <v>3875</v>
       </c>
       <c r="L8" s="5">
-        <v>4524</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -51773,36 +51767,36 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F9" s="5">
-        <v>880</v>
+        <v>1477</v>
       </c>
       <c r="G9" s="5">
-        <v>941</v>
+        <v>3957</v>
       </c>
       <c r="H9" s="5">
-        <v>2046</v>
+        <v>43556</v>
       </c>
       <c r="I9" s="5">
-        <v>1821</v>
+        <v>5434</v>
       </c>
       <c r="J9" s="5">
-        <v>11363</v>
+        <v>6770</v>
       </c>
       <c r="K9" s="5">
-        <v>10626</v>
+        <v>2527</v>
       </c>
       <c r="L9" s="5">
-        <v>5491</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
@@ -51814,33 +51808,33 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F10" s="5">
-        <v>230</v>
+        <v>64072</v>
       </c>
       <c r="G10" s="5">
-        <v>201</v>
+        <v>133585</v>
       </c>
       <c r="H10" s="5">
-        <v>2065</v>
+        <v>100127</v>
       </c>
       <c r="I10" s="5">
-        <v>431</v>
+        <v>197657</v>
       </c>
       <c r="J10" s="5">
-        <v>43478</v>
+        <v>156</v>
       </c>
       <c r="K10" s="5">
-        <v>49751</v>
+        <v>74</v>
       </c>
       <c r="L10" s="5">
-        <v>23201</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
@@ -51852,33 +51846,33 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F11" s="5">
-        <v>192</v>
+        <v>2518</v>
       </c>
       <c r="G11" s="5">
-        <v>198</v>
+        <v>2970</v>
       </c>
       <c r="H11" s="5">
-        <v>2046</v>
+        <v>100127</v>
       </c>
       <c r="I11" s="5">
-        <v>390</v>
+        <v>5488</v>
       </c>
       <c r="J11" s="5">
-        <v>52083</v>
+        <v>3971</v>
       </c>
       <c r="K11" s="5">
-        <v>50505</v>
+        <v>3367</v>
       </c>
       <c r="L11" s="5">
-        <v>25641</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
@@ -51887,36 +51881,36 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" s="5">
-        <v>201</v>
+        <v>1412</v>
       </c>
       <c r="G12" s="5">
-        <v>206</v>
+        <v>1796</v>
       </c>
       <c r="H12" s="5">
-        <v>2065</v>
+        <v>48468</v>
       </c>
       <c r="I12" s="5">
-        <v>407</v>
+        <v>3208</v>
       </c>
       <c r="J12" s="5">
-        <v>49751</v>
+        <v>7082</v>
       </c>
       <c r="K12" s="5">
-        <v>48543</v>
+        <v>5567</v>
       </c>
       <c r="L12" s="5">
-        <v>24570</v>
+        <v>3117</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
@@ -51925,31 +51919,31 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F13" s="5">
-        <v>188</v>
+        <v>1784</v>
       </c>
       <c r="G13" s="5">
-        <v>183</v>
+        <v>1165</v>
       </c>
       <c r="H13" s="5">
-        <v>2046</v>
+        <v>15032</v>
       </c>
       <c r="I13" s="5">
-        <v>371</v>
+        <v>2949</v>
       </c>
       <c r="J13" s="5">
-        <v>53191</v>
+        <v>5605</v>
       </c>
       <c r="K13" s="5">
-        <v>54644</v>
+        <v>8583</v>
       </c>
       <c r="L13" s="5">
-        <v>26954</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -51957,37 +51951,37 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="F14" s="5">
-        <v>18696</v>
+        <v>2703</v>
       </c>
       <c r="G14" s="5">
-        <v>4884</v>
+        <v>2459</v>
       </c>
       <c r="H14" s="5">
-        <v>2208</v>
+        <v>24128</v>
       </c>
       <c r="I14" s="5">
-        <v>23580</v>
+        <v>5162</v>
       </c>
       <c r="J14" s="5">
-        <v>534</v>
+        <v>3699</v>
       </c>
       <c r="K14" s="5">
-        <v>2047</v>
+        <v>4066</v>
       </c>
       <c r="L14" s="5">
-        <v>424</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -51995,37 +51989,37 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F15" s="5">
-        <v>41892</v>
+        <v>1443</v>
       </c>
       <c r="G15" s="5">
-        <v>24374</v>
+        <v>3696</v>
       </c>
       <c r="H15" s="5">
-        <v>1279</v>
+        <v>43556</v>
       </c>
       <c r="I15" s="5">
-        <v>66266</v>
+        <v>5139</v>
       </c>
       <c r="J15" s="5">
-        <v>238</v>
+        <v>6930</v>
       </c>
       <c r="K15" s="5">
-        <v>410</v>
+        <v>2705</v>
       </c>
       <c r="L15" s="5">
-        <v>150</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -52033,37 +52027,37 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F16" s="5">
-        <v>10625</v>
+        <v>65489</v>
       </c>
       <c r="G16" s="5">
-        <v>10707</v>
+        <v>126357</v>
       </c>
       <c r="H16" s="5">
-        <v>1136</v>
+        <v>100127</v>
       </c>
       <c r="I16" s="5">
-        <v>21332</v>
+        <v>191846</v>
       </c>
       <c r="J16" s="5">
-        <v>941</v>
+        <v>152</v>
       </c>
       <c r="K16" s="5">
-        <v>933</v>
+        <v>79</v>
       </c>
       <c r="L16" s="5">
-        <v>468</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -52071,37 +52065,37 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="F17" s="5">
-        <v>542</v>
+        <v>2535</v>
       </c>
       <c r="G17" s="5">
-        <v>541</v>
+        <v>4756</v>
       </c>
       <c r="H17" s="5">
-        <v>2208</v>
+        <v>100127</v>
       </c>
       <c r="I17" s="5">
-        <v>1083</v>
+        <v>7291</v>
       </c>
       <c r="J17" s="5">
-        <v>18450</v>
+        <v>3944</v>
       </c>
       <c r="K17" s="5">
-        <v>18484</v>
+        <v>2102</v>
       </c>
       <c r="L17" s="5">
-        <v>9233</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -52109,37 +52103,37 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F18" s="5">
-        <v>198</v>
+        <v>1437</v>
       </c>
       <c r="G18" s="5">
-        <v>246</v>
+        <v>1740</v>
       </c>
       <c r="H18" s="5">
-        <v>1279</v>
+        <v>48468</v>
       </c>
       <c r="I18" s="5">
-        <v>444</v>
+        <v>3177</v>
       </c>
       <c r="J18" s="5">
-        <v>50505</v>
+        <v>6958</v>
       </c>
       <c r="K18" s="5">
-        <v>40650</v>
+        <v>5747</v>
       </c>
       <c r="L18" s="5">
-        <v>22522</v>
+        <v>3147</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -52147,151 +52141,151 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F19" s="5">
-        <v>111</v>
+        <v>1733</v>
       </c>
       <c r="G19" s="5">
-        <v>124</v>
+        <v>1060</v>
       </c>
       <c r="H19" s="5">
-        <v>1136</v>
+        <v>15032</v>
       </c>
       <c r="I19" s="5">
-        <v>235</v>
+        <v>2793</v>
       </c>
       <c r="J19" s="5">
-        <v>90090</v>
+        <v>5770</v>
       </c>
       <c r="K19" s="5">
-        <v>80645</v>
+        <v>9433</v>
       </c>
       <c r="L19" s="5">
-        <v>42553</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="F20" s="5">
-        <v>373</v>
+        <v>2848</v>
       </c>
       <c r="G20" s="5">
-        <v>328</v>
+        <v>2412</v>
       </c>
       <c r="H20" s="5">
-        <v>2208</v>
+        <v>18096</v>
       </c>
       <c r="I20" s="5">
-        <v>701</v>
+        <v>5260</v>
       </c>
       <c r="J20" s="5">
-        <v>26809</v>
+        <v>3511</v>
       </c>
       <c r="K20" s="5">
-        <v>30487</v>
+        <v>4145</v>
       </c>
       <c r="L20" s="5">
-        <v>14265</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
         <v>2</v>
       </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
       <c r="F21" s="5">
-        <v>123</v>
+        <v>1347</v>
       </c>
       <c r="G21" s="5">
-        <v>135</v>
+        <v>3127</v>
       </c>
       <c r="H21" s="5">
-        <v>1279</v>
+        <v>32665</v>
       </c>
       <c r="I21" s="5">
-        <v>258</v>
+        <v>4474</v>
       </c>
       <c r="J21" s="5">
-        <v>81300</v>
+        <v>7423</v>
       </c>
       <c r="K21" s="5">
-        <v>74074</v>
+        <v>3197</v>
       </c>
       <c r="L21" s="5">
-        <v>38759</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F22" s="5">
-        <v>106</v>
+        <v>1444</v>
       </c>
       <c r="G22" s="5">
-        <v>129</v>
+        <v>1382</v>
       </c>
       <c r="H22" s="5">
-        <v>1136</v>
+        <v>36349</v>
       </c>
       <c r="I22" s="5">
-        <v>235</v>
+        <v>2826</v>
       </c>
       <c r="J22" s="5">
-        <v>94339</v>
+        <v>6925</v>
       </c>
       <c r="K22" s="5">
-        <v>77519</v>
+        <v>7235</v>
       </c>
       <c r="L22" s="5">
-        <v>42553</v>
+        <v>3538</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -52299,7 +52293,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -52308,28 +52302,28 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="F23" s="5">
-        <v>328</v>
+        <v>1882</v>
       </c>
       <c r="G23" s="5">
-        <v>273</v>
+        <v>1136</v>
       </c>
       <c r="H23" s="5">
-        <v>1654</v>
+        <v>11272</v>
       </c>
       <c r="I23" s="5">
-        <v>601</v>
+        <v>3018</v>
       </c>
       <c r="J23" s="5">
-        <v>30487</v>
+        <v>5313</v>
       </c>
       <c r="K23" s="5">
-        <v>36630</v>
+        <v>8802</v>
       </c>
       <c r="L23" s="5">
-        <v>16638</v>
+        <v>3313</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -52337,37 +52331,37 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F24" s="5">
-        <v>114</v>
+        <v>2735</v>
       </c>
       <c r="G24" s="5">
-        <v>155</v>
+        <v>2172</v>
       </c>
       <c r="H24" s="5">
-        <v>1279</v>
+        <v>18096</v>
       </c>
       <c r="I24" s="5">
-        <v>269</v>
+        <v>4907</v>
       </c>
       <c r="J24" s="5">
-        <v>87719</v>
+        <v>3656</v>
       </c>
       <c r="K24" s="5">
-        <v>64516</v>
+        <v>4604</v>
       </c>
       <c r="L24" s="5">
-        <v>37174</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -52375,37 +52369,37 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F25" s="5">
-        <v>117</v>
+        <v>1221</v>
       </c>
       <c r="G25" s="5">
-        <v>151</v>
+        <v>3225</v>
       </c>
       <c r="H25" s="5">
-        <v>1136</v>
+        <v>32665</v>
       </c>
       <c r="I25" s="5">
-        <v>268</v>
+        <v>4446</v>
       </c>
       <c r="J25" s="5">
-        <v>85470</v>
+        <v>8190</v>
       </c>
       <c r="K25" s="5">
-        <v>66225</v>
+        <v>3100</v>
       </c>
       <c r="L25" s="5">
-        <v>37313</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -52413,7 +52407,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -52422,28 +52416,28 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="F26" s="5">
-        <v>510</v>
+        <v>1218</v>
       </c>
       <c r="G26" s="5">
-        <v>407</v>
+        <v>1159</v>
       </c>
       <c r="H26" s="5">
-        <v>1654</v>
+        <v>36349</v>
       </c>
       <c r="I26" s="5">
-        <v>917</v>
+        <v>2377</v>
       </c>
       <c r="J26" s="5">
-        <v>19607</v>
+        <v>8210</v>
       </c>
       <c r="K26" s="5">
-        <v>24570</v>
+        <v>8628</v>
       </c>
       <c r="L26" s="5">
-        <v>10905</v>
+        <v>4206</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -52451,7 +52445,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -52460,28 +52454,28 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27" s="5">
-        <v>99</v>
+        <v>1705</v>
       </c>
       <c r="G27" s="5">
-        <v>207</v>
+        <v>1295</v>
       </c>
       <c r="H27" s="5">
-        <v>1279</v>
+        <v>11272</v>
       </c>
       <c r="I27" s="5">
-        <v>306</v>
+        <v>3000</v>
       </c>
       <c r="J27" s="5">
-        <v>101010</v>
+        <v>5865</v>
       </c>
       <c r="K27" s="5">
-        <v>48309</v>
+        <v>7722</v>
       </c>
       <c r="L27" s="5">
-        <v>32679</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -52489,37 +52483,37 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
       <c r="F28" s="5">
-        <v>145</v>
+        <v>2716</v>
       </c>
       <c r="G28" s="5">
-        <v>186</v>
+        <v>2202</v>
       </c>
       <c r="H28" s="5">
-        <v>1136</v>
+        <v>18096</v>
       </c>
       <c r="I28" s="5">
-        <v>331</v>
+        <v>4918</v>
       </c>
       <c r="J28" s="5">
-        <v>68965</v>
+        <v>3681</v>
       </c>
       <c r="K28" s="5">
-        <v>53763</v>
+        <v>4541</v>
       </c>
       <c r="L28" s="5">
-        <v>30211</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -52527,7 +52521,7 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -52536,28 +52530,28 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="F29" s="5">
-        <v>418</v>
+        <v>1229</v>
       </c>
       <c r="G29" s="5">
-        <v>344</v>
+        <v>2890</v>
       </c>
       <c r="H29" s="5">
-        <v>1654</v>
+        <v>32665</v>
       </c>
       <c r="I29" s="5">
-        <v>762</v>
+        <v>4119</v>
       </c>
       <c r="J29" s="5">
-        <v>23923</v>
+        <v>8136</v>
       </c>
       <c r="K29" s="5">
-        <v>29069</v>
+        <v>3460</v>
       </c>
       <c r="L29" s="5">
-        <v>13123</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -52565,7 +52559,7 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -52574,28 +52568,28 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F30" s="5">
-        <v>120</v>
+        <v>1250</v>
       </c>
       <c r="G30" s="5">
-        <v>166</v>
+        <v>1157</v>
       </c>
       <c r="H30" s="5">
-        <v>1279</v>
+        <v>36349</v>
       </c>
       <c r="I30" s="5">
-        <v>286</v>
+        <v>2407</v>
       </c>
       <c r="J30" s="5">
-        <v>83333</v>
+        <v>8000</v>
       </c>
       <c r="K30" s="5">
-        <v>60240</v>
+        <v>8643</v>
       </c>
       <c r="L30" s="5">
-        <v>34965</v>
+        <v>4154</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -52603,7 +52597,7 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -52612,28 +52606,28 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F31" s="5">
-        <v>164</v>
+        <v>1652</v>
       </c>
       <c r="G31" s="5">
-        <v>205</v>
+        <v>1381</v>
       </c>
       <c r="H31" s="5">
-        <v>1136</v>
+        <v>11272</v>
       </c>
       <c r="I31" s="5">
-        <v>369</v>
+        <v>3033</v>
       </c>
       <c r="J31" s="5">
-        <v>60975</v>
+        <v>6053</v>
       </c>
       <c r="K31" s="5">
-        <v>48780</v>
+        <v>7241</v>
       </c>
       <c r="L31" s="5">
-        <v>27100</v>
+        <v>3297</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -52641,7 +52635,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -52650,28 +52644,28 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F32" s="5">
-        <v>208519</v>
+        <v>2820</v>
       </c>
       <c r="G32" s="5">
-        <v>157763</v>
+        <v>2536</v>
       </c>
       <c r="H32" s="5">
-        <v>25065</v>
+        <v>24128</v>
       </c>
       <c r="I32" s="5">
-        <v>366282</v>
+        <v>5356</v>
       </c>
       <c r="J32" s="5">
-        <v>47</v>
+        <v>3546</v>
       </c>
       <c r="K32" s="5">
-        <v>63</v>
+        <v>3943</v>
       </c>
       <c r="L32" s="5">
-        <v>27</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -52679,7 +52673,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -52688,28 +52682,28 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F33" s="5">
-        <v>119862</v>
+        <v>1448</v>
       </c>
       <c r="G33" s="5">
-        <v>111399</v>
+        <v>3599</v>
       </c>
       <c r="H33" s="5">
-        <v>22221</v>
+        <v>43556</v>
       </c>
       <c r="I33" s="5">
-        <v>231261</v>
+        <v>5047</v>
       </c>
       <c r="J33" s="5">
-        <v>83</v>
+        <v>6906</v>
       </c>
       <c r="K33" s="5">
-        <v>89</v>
+        <v>2778</v>
       </c>
       <c r="L33" s="5">
-        <v>43</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -52717,37 +52711,37 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F34" s="5">
-        <v>842</v>
+        <v>65698</v>
       </c>
       <c r="G34" s="5">
-        <v>2325</v>
+        <v>120488</v>
       </c>
       <c r="H34" s="5">
-        <v>25065</v>
+        <v>100127</v>
       </c>
       <c r="I34" s="5">
-        <v>3167</v>
+        <v>186186</v>
       </c>
       <c r="J34" s="5">
-        <v>11876</v>
+        <v>152</v>
       </c>
       <c r="K34" s="5">
-        <v>4301</v>
+        <v>82</v>
       </c>
       <c r="L34" s="5">
-        <v>3157</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -52755,37 +52749,37 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F35" s="5">
-        <v>830</v>
+        <v>2453</v>
       </c>
       <c r="G35" s="5">
-        <v>1985</v>
+        <v>2873</v>
       </c>
       <c r="H35" s="5">
-        <v>22221</v>
+        <v>100127</v>
       </c>
       <c r="I35" s="5">
-        <v>2815</v>
+        <v>5326</v>
       </c>
       <c r="J35" s="5">
-        <v>12048</v>
+        <v>4076</v>
       </c>
       <c r="K35" s="5">
-        <v>5037</v>
+        <v>3480</v>
       </c>
       <c r="L35" s="5">
-        <v>3552</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -52793,37 +52787,37 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>3</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F36" s="5">
-        <v>875</v>
+        <v>1415</v>
       </c>
       <c r="G36" s="5">
-        <v>2476</v>
+        <v>2563</v>
       </c>
       <c r="H36" s="5">
-        <v>25065</v>
+        <v>48468</v>
       </c>
       <c r="I36" s="5">
-        <v>3351</v>
+        <v>3978</v>
       </c>
       <c r="J36" s="5">
-        <v>11428</v>
+        <v>7067</v>
       </c>
       <c r="K36" s="5">
-        <v>4038</v>
+        <v>3901</v>
       </c>
       <c r="L36" s="5">
-        <v>2984</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -52831,121 +52825,121 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F37" s="5">
-        <v>805</v>
+        <v>1636</v>
       </c>
       <c r="G37" s="5">
-        <v>1974</v>
+        <v>1119</v>
       </c>
       <c r="H37" s="5">
-        <v>22221</v>
+        <v>15032</v>
       </c>
       <c r="I37" s="5">
-        <v>2779</v>
+        <v>2755</v>
       </c>
       <c r="J37" s="5">
-        <v>12422</v>
+        <v>6112</v>
       </c>
       <c r="K37" s="5">
-        <v>5065</v>
+        <v>8936</v>
       </c>
       <c r="L37" s="5">
-        <v>3598</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F38" s="5">
-        <v>972</v>
+        <v>2821</v>
       </c>
       <c r="G38" s="5">
-        <v>2544</v>
+        <v>3647</v>
       </c>
       <c r="H38" s="5">
-        <v>25065</v>
+        <v>24128</v>
       </c>
       <c r="I38" s="5">
-        <v>3516</v>
+        <v>6468</v>
       </c>
       <c r="J38" s="5">
-        <v>10288</v>
+        <v>3544</v>
       </c>
       <c r="K38" s="5">
-        <v>3930</v>
+        <v>2741</v>
       </c>
       <c r="L38" s="5">
-        <v>2844</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F39" s="5">
-        <v>898</v>
+        <v>1485</v>
       </c>
       <c r="G39" s="5">
-        <v>2190</v>
+        <v>3412</v>
       </c>
       <c r="H39" s="5">
-        <v>22221</v>
+        <v>43556</v>
       </c>
       <c r="I39" s="5">
-        <v>3088</v>
+        <v>4897</v>
       </c>
       <c r="J39" s="5">
-        <v>11135</v>
+        <v>6734</v>
       </c>
       <c r="K39" s="5">
-        <v>4566</v>
+        <v>2930</v>
       </c>
       <c r="L39" s="5">
-        <v>3238</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -52954,36 +52948,36 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F40" s="5">
-        <v>896</v>
+        <v>65197</v>
       </c>
       <c r="G40" s="5">
-        <v>2464</v>
+        <v>125979</v>
       </c>
       <c r="H40" s="5">
-        <v>25065</v>
+        <v>100127</v>
       </c>
       <c r="I40" s="5">
-        <v>3360</v>
+        <v>191176</v>
       </c>
       <c r="J40" s="5">
-        <v>11160</v>
+        <v>153</v>
       </c>
       <c r="K40" s="5">
-        <v>4058</v>
+        <v>79</v>
       </c>
       <c r="L40" s="5">
-        <v>2976</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -52992,104 +52986,788 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F41" s="5">
-        <v>827</v>
+        <v>2525</v>
       </c>
       <c r="G41" s="5">
-        <v>1933</v>
+        <v>3015</v>
       </c>
       <c r="H41" s="5">
-        <v>22221</v>
+        <v>100127</v>
       </c>
       <c r="I41" s="5">
-        <v>2760</v>
+        <v>5540</v>
       </c>
       <c r="J41" s="5">
-        <v>12091</v>
+        <v>3960</v>
       </c>
       <c r="K41" s="5">
-        <v>5173</v>
+        <v>3316</v>
       </c>
       <c r="L41" s="5">
-        <v>3623</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C42">
         <v>3</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F42" s="5">
-        <v>871</v>
+        <v>1519</v>
       </c>
       <c r="G42" s="5">
-        <v>2458</v>
+        <v>1881</v>
       </c>
       <c r="H42" s="5">
-        <v>25065</v>
+        <v>48468</v>
       </c>
       <c r="I42" s="5">
-        <v>3329</v>
+        <v>3400</v>
       </c>
       <c r="J42" s="5">
-        <v>11481</v>
+        <v>6583</v>
       </c>
       <c r="K42" s="5">
-        <v>4068</v>
+        <v>5316</v>
       </c>
       <c r="L42" s="5">
-        <v>3003</v>
+        <v>2941</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C43">
         <v>3</v>
       </c>
       <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="5">
+        <v>1791</v>
+      </c>
+      <c r="G43" s="5">
+        <v>1141</v>
+      </c>
+      <c r="H43" s="5">
+        <v>15032</v>
+      </c>
+      <c r="I43" s="5">
+        <v>2932</v>
+      </c>
+      <c r="J43" s="5">
+        <v>5583</v>
+      </c>
+      <c r="K43" s="5">
+        <v>8764</v>
+      </c>
+      <c r="L43" s="5">
+        <v>3410</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
         <v>2</v>
       </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" s="5">
+      <c r="E44" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="5">
+        <v>3277</v>
+      </c>
+      <c r="G44" s="5">
+        <v>2542</v>
+      </c>
+      <c r="H44" s="5">
+        <v>24128</v>
+      </c>
+      <c r="I44" s="5">
+        <v>5819</v>
+      </c>
+      <c r="J44" s="5">
+        <v>3051</v>
+      </c>
+      <c r="K44" s="5">
+        <v>3933</v>
+      </c>
+      <c r="L44" s="5">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="5">
+        <v>2433</v>
+      </c>
+      <c r="G45" s="5">
+        <v>3690</v>
+      </c>
+      <c r="H45" s="5">
+        <v>43556</v>
+      </c>
+      <c r="I45" s="5">
+        <v>6123</v>
+      </c>
+      <c r="J45" s="5">
+        <v>4110</v>
+      </c>
+      <c r="K45" s="5">
+        <v>2710</v>
+      </c>
+      <c r="L45" s="5">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="5">
+        <v>63832</v>
+      </c>
+      <c r="G46" s="5">
+        <v>125924</v>
+      </c>
+      <c r="H46" s="5">
+        <v>100127</v>
+      </c>
+      <c r="I46" s="5">
+        <v>189756</v>
+      </c>
+      <c r="J46" s="5">
+        <v>156</v>
+      </c>
+      <c r="K46" s="5">
+        <v>79</v>
+      </c>
+      <c r="L46" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="5">
+        <v>2414</v>
+      </c>
+      <c r="G47" s="5">
+        <v>2793</v>
+      </c>
+      <c r="H47" s="5">
+        <v>100127</v>
+      </c>
+      <c r="I47" s="5">
+        <v>5207</v>
+      </c>
+      <c r="J47" s="5">
+        <v>4142</v>
+      </c>
+      <c r="K47" s="5">
+        <v>3580</v>
+      </c>
+      <c r="L47" s="5">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1465</v>
+      </c>
+      <c r="G48" s="5">
+        <v>1870</v>
+      </c>
+      <c r="H48" s="5">
+        <v>48468</v>
+      </c>
+      <c r="I48" s="5">
+        <v>3335</v>
+      </c>
+      <c r="J48" s="5">
+        <v>6825</v>
+      </c>
+      <c r="K48" s="5">
+        <v>5347</v>
+      </c>
+      <c r="L48" s="5">
+        <v>2998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="5">
+        <v>1748</v>
+      </c>
+      <c r="G49" s="5">
+        <v>1145</v>
+      </c>
+      <c r="H49" s="5">
+        <v>15032</v>
+      </c>
+      <c r="I49" s="5">
+        <v>2893</v>
+      </c>
+      <c r="J49" s="5">
+        <v>5720</v>
+      </c>
+      <c r="K49" s="5">
+        <v>8733</v>
+      </c>
+      <c r="L49" s="5">
+        <v>3456</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="5">
+        <v>3282</v>
+      </c>
+      <c r="G50" s="5">
+        <v>2264</v>
+      </c>
+      <c r="H50" s="5">
+        <v>18096</v>
+      </c>
+      <c r="I50" s="5">
+        <v>5546</v>
+      </c>
+      <c r="J50" s="5">
+        <v>3046</v>
+      </c>
+      <c r="K50" s="5">
+        <v>4416</v>
+      </c>
+      <c r="L50" s="5">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" s="5">
+        <v>1195</v>
+      </c>
+      <c r="G51" s="5">
+        <v>2897</v>
+      </c>
+      <c r="H51" s="5">
+        <v>32665</v>
+      </c>
+      <c r="I51" s="5">
+        <v>4092</v>
+      </c>
+      <c r="J51" s="5">
+        <v>8368</v>
+      </c>
+      <c r="K51" s="5">
+        <v>3451</v>
+      </c>
+      <c r="L51" s="5">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="5">
+        <v>1082</v>
+      </c>
+      <c r="G52" s="5">
+        <v>1085</v>
+      </c>
+      <c r="H52" s="5">
+        <v>36349</v>
+      </c>
+      <c r="I52" s="5">
+        <v>2167</v>
+      </c>
+      <c r="J52" s="5">
+        <v>9242</v>
+      </c>
+      <c r="K52" s="5">
+        <v>9216</v>
+      </c>
+      <c r="L52" s="5">
+        <v>4614</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="5">
+        <v>1515</v>
+      </c>
+      <c r="G53" s="5">
         <v>842</v>
       </c>
-      <c r="G43" s="5">
-        <v>1953</v>
-      </c>
-      <c r="H43" s="5">
-        <v>22221</v>
-      </c>
-      <c r="I43" s="5">
-        <v>2795</v>
-      </c>
-      <c r="J43" s="5">
+      <c r="H53" s="5">
+        <v>11272</v>
+      </c>
+      <c r="I53" s="5">
+        <v>2357</v>
+      </c>
+      <c r="J53" s="5">
+        <v>6600</v>
+      </c>
+      <c r="K53" s="5">
         <v>11876</v>
       </c>
-      <c r="K43" s="5">
-        <v>5120</v>
-      </c>
-      <c r="L43" s="5">
-        <v>3577</v>
+      <c r="L53" s="5">
+        <v>4242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" s="5">
+        <v>3058</v>
+      </c>
+      <c r="G54" s="5">
+        <v>2331</v>
+      </c>
+      <c r="H54" s="5">
+        <v>18096</v>
+      </c>
+      <c r="I54" s="5">
+        <v>5389</v>
+      </c>
+      <c r="J54" s="5">
+        <v>3270</v>
+      </c>
+      <c r="K54" s="5">
+        <v>4290</v>
+      </c>
+      <c r="L54" s="5">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="5">
+        <v>1246</v>
+      </c>
+      <c r="G55" s="5">
+        <v>3111</v>
+      </c>
+      <c r="H55" s="5">
+        <v>32665</v>
+      </c>
+      <c r="I55" s="5">
+        <v>4357</v>
+      </c>
+      <c r="J55" s="5">
+        <v>8025</v>
+      </c>
+      <c r="K55" s="5">
+        <v>3214</v>
+      </c>
+      <c r="L55" s="5">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="5">
+        <v>1231</v>
+      </c>
+      <c r="G56" s="5">
+        <v>1151</v>
+      </c>
+      <c r="H56" s="5">
+        <v>36349</v>
+      </c>
+      <c r="I56" s="5">
+        <v>2382</v>
+      </c>
+      <c r="J56" s="5">
+        <v>8123</v>
+      </c>
+      <c r="K56" s="5">
+        <v>8688</v>
+      </c>
+      <c r="L56" s="5">
+        <v>4198</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="5">
+        <v>1599</v>
+      </c>
+      <c r="G57" s="5">
+        <v>865</v>
+      </c>
+      <c r="H57" s="5">
+        <v>11272</v>
+      </c>
+      <c r="I57" s="5">
+        <v>2464</v>
+      </c>
+      <c r="J57" s="5">
+        <v>6253</v>
+      </c>
+      <c r="K57" s="5">
+        <v>11560</v>
+      </c>
+      <c r="L57" s="5">
+        <v>4058</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="5">
+        <v>2705</v>
+      </c>
+      <c r="G58" s="5">
+        <v>2183</v>
+      </c>
+      <c r="H58" s="5">
+        <v>18096</v>
+      </c>
+      <c r="I58" s="5">
+        <v>4888</v>
+      </c>
+      <c r="J58" s="5">
+        <v>3696</v>
+      </c>
+      <c r="K58" s="5">
+        <v>4580</v>
+      </c>
+      <c r="L58" s="5">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="5">
+        <v>1198</v>
+      </c>
+      <c r="G59" s="5">
+        <v>2894</v>
+      </c>
+      <c r="H59" s="5">
+        <v>32665</v>
+      </c>
+      <c r="I59" s="5">
+        <v>4092</v>
+      </c>
+      <c r="J59" s="5">
+        <v>8347</v>
+      </c>
+      <c r="K59" s="5">
+        <v>3455</v>
+      </c>
+      <c r="L59" s="5">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="5">
+        <v>1176</v>
+      </c>
+      <c r="G60" s="5">
+        <v>1085</v>
+      </c>
+      <c r="H60" s="5">
+        <v>36349</v>
+      </c>
+      <c r="I60" s="5">
+        <v>2261</v>
+      </c>
+      <c r="J60" s="5">
+        <v>8503</v>
+      </c>
+      <c r="K60" s="5">
+        <v>9216</v>
+      </c>
+      <c r="L60" s="5">
+        <v>4422</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="5">
+        <v>1544</v>
+      </c>
+      <c r="G61" s="5">
+        <v>813</v>
+      </c>
+      <c r="H61" s="5">
+        <v>11272</v>
+      </c>
+      <c r="I61" s="5">
+        <v>2357</v>
+      </c>
+      <c r="J61" s="5">
+        <v>6476</v>
+      </c>
+      <c r="K61" s="5">
+        <v>12300</v>
+      </c>
+      <c r="L61" s="5">
+        <v>4242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>